<commit_message>
Changed hyper contractility to hypo
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5BF153-7C11-42F0-9623-4BD153261970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4402CE-2BC4-4BBB-94D8-A5A50C85E684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Anal hypotension with normal contractility</t>
   </si>
   <si>
-    <t>Anal normotension with hypercontractility</t>
-  </si>
-  <si>
     <t>No disorder of anal tone and contractility</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Hypo; normal contractility</t>
   </si>
   <si>
-    <t>Norm; hypercontractility</t>
-  </si>
-  <si>
     <t>Abn  ex; poor propulsion</t>
   </si>
   <si>
@@ -225,6 +219,12 @@
   </si>
   <si>
     <t>Addition of an abnormal cough response may indicate a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but its use as a diagnostic criterion is unproven.</t>
+  </si>
+  <si>
+    <t>Anal normotension with hypocontractility</t>
+  </si>
+  <si>
+    <t>Norm; hypocontractility</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -581,36 +581,36 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -630,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -647,19 +647,19 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -670,19 +670,19 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -693,22 +693,22 @@
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>0.6</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -728,13 +728,13 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7">
         <v>1.4</v>
@@ -745,16 +745,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -765,19 +765,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -788,19 +788,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -811,19 +811,19 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -834,22 +834,22 @@
     </row>
     <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -860,19 +860,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -883,19 +883,19 @@
     </row>
     <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -906,16 +906,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -926,16 +926,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -946,19 +946,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17">
         <v>3</v>
@@ -969,19 +969,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -992,16 +992,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -1012,19 +1012,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1035,19 +1035,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -1058,16 +1058,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1078,19 +1078,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1101,19 +1101,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1170,13 +1170,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1193,12 +1193,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1207,12 +1207,12 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1221,12 +1221,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1235,12 +1235,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1249,12 +1249,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1263,12 +1263,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1277,12 +1277,12 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1291,12 +1291,12 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1305,12 +1305,12 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1319,12 +1319,12 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1333,12 +1333,12 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1347,12 +1347,12 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1361,12 +1361,12 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1375,12 +1375,12 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1389,12 +1389,12 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1403,12 +1403,12 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1417,12 +1417,12 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1431,12 +1431,12 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1445,12 +1445,12 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1459,7 +1459,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed invalid print(group) Unhide danger zone for testing Do not load admin module for non-admin users Disable Record selection in admin mode README credits read from DESCRIPTION Version 1.25 Typo in node_edges.
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4402CE-2BC4-4BBB-94D8-A5A50C85E684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAF28C2-6199-473A-A10D-55485E819565}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Addition of an abnormal cough response may indicated a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but ist use as a diagnostic criterion is unproven.</t>
-  </si>
-  <si>
-    <t>The value of LLL (lower limit of normal ULN) is not yet defined.</t>
   </si>
   <si>
     <t>Anal hypotension with normal contractility</t>
@@ -215,9 +212,6 @@
     <t>Anal resting pressure &gt; ULN</t>
   </si>
   <si>
-    <t>Anal squeeze pressure &gt; LLN</t>
-  </si>
-  <si>
     <t>Addition of an abnormal cough response may indicate a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but its use as a diagnostic criterion is unproven.</t>
   </si>
   <si>
@@ -225,6 +219,9 @@
   </si>
   <si>
     <t>Norm; hypocontractility</t>
+  </si>
+  <si>
+    <t>The value of LLN (lower limit of normal ULN) is not yet defined.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +551,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -572,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -581,36 +578,36 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -621,7 +618,7 @@
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -630,13 +627,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -647,19 +644,19 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -670,19 +667,19 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -693,22 +690,22 @@
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>0.6</v>
@@ -719,22 +716,22 @@
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>1.4</v>
@@ -745,16 +742,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -765,19 +762,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -788,19 +785,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -811,19 +808,19 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -834,22 +831,22 @@
     </row>
     <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -860,19 +857,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -883,19 +880,19 @@
     </row>
     <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -906,16 +903,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -926,16 +923,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -946,19 +943,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17">
         <v>3</v>
@@ -969,19 +966,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -992,16 +989,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -1012,19 +1009,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1035,19 +1032,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -1058,16 +1055,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1078,19 +1075,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1101,19 +1098,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1170,13 +1167,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1184,7 +1181,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1193,12 +1190,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1207,12 +1204,12 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1221,12 +1218,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1235,12 +1232,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1249,12 +1246,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1263,12 +1260,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1277,12 +1274,12 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1291,12 +1288,12 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1305,12 +1302,12 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1319,12 +1316,12 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1333,12 +1330,12 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1347,12 +1344,12 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1361,12 +1358,12 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1375,12 +1372,12 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1389,12 +1386,12 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1403,12 +1400,12 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1417,12 +1414,12 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1431,12 +1428,12 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1445,12 +1442,12 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1459,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected typo in node_edges.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAF28C2-6199-473A-A10D-55485E819565}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DBC79E-1B2C-4F10-82AA-D32410A2DD6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>The functional anal canal length may be measured, as a short anal canal can be associated with anal hypotonia, but its use as a diagnostic criterion in isolation is unproven.</t>
   </si>
   <si>
-    <t>Addition of an abnormal cough response may indicated a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but ist use as a diagnostic criterion is unproven.</t>
-  </si>
-  <si>
     <t>Anal hypotension with normal contractility</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>The value of LLN (lower limit of normal ULN) is not yet defined.</t>
+  </si>
+  <si>
+    <t>Addition of an abnormal cough response may indicated a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but its use as a diagnostic criterion is unproven.</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -578,36 +578,36 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -627,13 +627,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -644,19 +644,19 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -667,19 +667,19 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -690,22 +690,22 @@
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0.6</v>
@@ -716,22 +716,22 @@
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>1.4</v>
@@ -742,16 +742,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -762,19 +762,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -785,19 +785,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -808,19 +808,19 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -831,22 +831,22 @@
     </row>
     <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -857,19 +857,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -880,19 +880,19 @@
     </row>
     <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -903,16 +903,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -923,16 +923,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -943,19 +943,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>3</v>
@@ -966,19 +966,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -989,16 +989,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -1009,19 +1009,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -1032,19 +1032,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -1055,16 +1055,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1075,19 +1075,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1098,19 +1098,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1167,13 +1167,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1190,12 +1190,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1204,12 +1204,12 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1218,12 +1218,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1232,12 +1232,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1246,12 +1246,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1260,12 +1260,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1274,12 +1274,12 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1288,12 +1288,12 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1302,12 +1302,12 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1316,12 +1316,12 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1330,12 +1330,12 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1344,12 +1344,12 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1358,12 +1358,12 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1372,12 +1372,12 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1386,12 +1386,12 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1400,12 +1400,12 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1414,12 +1414,12 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1428,12 +1428,12 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1442,12 +1442,12 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1456,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Protect against invalid show of expert ratings due to priority problem in app_server
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DBC79E-1B2C-4F10-82AA-D32410A2DD6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDF531-A2C0-5B43-872E-D5C70C7BB605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Rectal pressure increase during push &gt; LLN</t>
   </si>
   <si>
-    <t>Anal pressure decrease (relaxation) during push &gt; LLN</t>
-  </si>
-  <si>
     <t>Abnormal expulsion with normal manometric pattern of rectoanal coordination</t>
   </si>
   <si>
@@ -222,6 +219,12 @@
   </si>
   <si>
     <t>Addition of an abnormal cough response may indicated a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but its use as a diagnostic criterion is unproven.</t>
+  </si>
+  <si>
+    <t>Positive RAPG* / Anal pressure decrease (relaxation) during push &gt; LLN</t>
+  </si>
+  <si>
+    <t>* recto-anal pressure gradient (RAPG)</t>
   </si>
 </sst>
 </file>
@@ -548,26 +551,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" hidden="1"/>
+    <col min="13" max="16384" width="9.1640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -578,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -593,7 +596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -601,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -616,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -627,7 +630,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -642,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -665,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -676,7 +679,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -688,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -696,13 +699,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -714,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -725,10 +728,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -740,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -760,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -768,10 +771,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -783,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -794,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -806,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -829,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -840,7 +843,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>26</v>
@@ -855,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -866,7 +869,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -878,9 +881,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -889,7 +892,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -901,9 +904,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -921,15 +924,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -941,18 +944,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -964,18 +967,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -987,15 +990,15 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1007,18 +1010,18 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
         <v>15</v>
@@ -1030,18 +1033,18 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -1053,15 +1056,15 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
@@ -1073,18 +1076,18 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -1096,18 +1099,18 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -1119,30 +1122,18 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1155,17 +1146,17 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" hidden="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1193,7 +1184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1207,7 +1198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +1212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1235,7 +1226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1249,7 +1240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1263,7 +1254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1277,7 +1268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1291,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1319,9 +1310,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1333,9 +1324,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1347,9 +1338,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1361,9 +1352,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1375,9 +1366,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1389,9 +1380,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1403,9 +1394,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1417,9 +1408,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1431,9 +1422,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1445,9 +1436,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1459,25 +1450,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="33" x14ac:dyDescent="0.25"/>
-    <row r="34" x14ac:dyDescent="0.25"/>
-    <row r="35" x14ac:dyDescent="0.25"/>
-    <row r="36" x14ac:dyDescent="0.25"/>
-    <row r="37" x14ac:dyDescent="0.25"/>
-    <row r="38" x14ac:dyDescent="0.25"/>
-    <row r="39" x14ac:dyDescent="0.25"/>
-    <row r="40" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="33" x14ac:dyDescent="0.2"/>
+    <row r="34" x14ac:dyDescent="0.2"/>
+    <row r="35" x14ac:dyDescent="0.2"/>
+    <row r="36" x14ac:dyDescent="0.2"/>
+    <row r="37" x14ac:dyDescent="0.2"/>
+    <row r="38" x14ac:dyDescent="0.2"/>
+    <row r="39" x14ac:dyDescent="0.2"/>
+    <row r="40" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected names for expert_classification; edited nodes_edges.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDF531-A2C0-5B43-872E-D5C70C7BB605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B0F08D-A40D-4783-95F2-CB58B8D7FA70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -221,10 +221,10 @@
     <t>Addition of an abnormal cough response may indicated a  more severe phenotype, whereas preservatation may suggest a target for biofeedback, but its use as a diagnostic criterion is unproven.</t>
   </si>
   <si>
-    <t>Positive RAPG* / Anal pressure decrease (relaxation) during push &gt; LLN</t>
-  </si>
-  <si>
-    <t>* recto-anal pressure gradient (RAPG)</t>
+    <t>Positive recto-anal pressure gradient (RAPG) / Anal pressure decrease (relaxation) during push &gt; LLN</t>
+  </si>
+  <si>
+    <t>Positive recto-anal pressure gradient (RAPG)/ Anal pressure decrease (relaxation) during push &gt; LLN</t>
   </si>
 </sst>
 </file>
@@ -553,24 +553,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" hidden="1"/>
+    <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -596,7 +596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -645,7 +645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -691,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -743,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -858,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -904,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -990,7 +990,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1010,7 +1010,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1122,15 +1122,11 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1146,17 +1142,17 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" hidden="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1170,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1184,7 +1180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1212,7 +1208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1226,7 +1222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1240,7 +1236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1282,7 +1278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1310,7 +1306,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1338,7 +1334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1352,7 +1348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1380,7 +1376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1394,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1408,7 +1404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1422,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1450,25 +1446,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected test database creation Version 1.6.1
Updated scripts

Uploaded 1.6

Removed experimental bookmarking
Removed all restrictions given warnings for rair and tone.
Updated node-edges.xlsx

Added reminder in case of inconsistent ratings.

Changed visible trainee to participant (internally, it's still trainee)

Corrected color status

Corrected imputation

Clinical and majority arrows

Test passed

Adding imputation

Several dplyr:: made global

Added update_expert_classification

Drop raw/cleaned tables if one does not exists

added clinical overrides

Partially working Update record items function

Added conflicted_prefer. Corrected display of labels in case of different clinical diagnosis

updated tests

Removed nodes in sysdata, replaced by automatic read from Excel and keep in database
</commit_message>
<xml_diff>
--- a/data-raw/nodes_edges.xlsx
+++ b/data-raw/nodes_edges.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EDF531-A2C0-5B43-872E-D5C70C7BB605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87413095-E8E9-436B-AA31-FFB64BB2F7D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Positive RAPG* / Anal pressure decrease (relaxation) during push &gt; LLN</t>
-  </si>
-  <si>
-    <t>* recto-anal pressure gradient (RAPG)</t>
   </si>
 </sst>
 </file>
@@ -553,24 +550,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="8" width="4" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" hidden="1"/>
+    <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -596,7 +593,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -619,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -645,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -668,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -691,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -717,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -743,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -763,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -786,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -809,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -832,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -858,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -881,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -904,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -924,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -944,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -967,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -990,7 +987,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1010,7 +1007,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1056,7 +1053,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1122,15 +1119,11 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1146,17 +1139,17 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" hidden="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1170,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1184,7 +1177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1212,7 +1205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1226,7 +1219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1240,7 +1233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1282,7 +1275,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1310,7 +1303,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1338,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1352,7 +1345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1380,7 +1373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1394,7 +1387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1408,7 +1401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1422,7 +1415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1436,7 +1429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1450,25 +1443,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2"/>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>